<commit_message>
Adiciona inicio da API
</commit_message>
<xml_diff>
--- a/reforco/tarde/lovePets/sprint-1-bd/modelagens/lovePets_modelagem-fisico.xlsx
+++ b/reforco/tarde/lovePets/sprint-1-bd/modelagens/lovePets_modelagem-fisico.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.santos\Downloads\SENAI\CT\2021-1S-2D\senai-dev-1s2021-alunos\reforco\tarde\lovePets\sprint-1-bd\modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD1BEF9-96C8-40A0-A2B0-6BE1F2C2F091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DE60C2-D1E5-4161-939C-4A3F11ABEEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2DD19EB1-C38B-4F91-8F06-CFED0BB47B4A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="lovePets" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>clinica</t>
   </si>
@@ -163,13 +163,100 @@
   </si>
   <si>
     <t>o paciente está ok</t>
+  </si>
+  <si>
+    <t>tipoUsuario</t>
+  </si>
+  <si>
+    <t>idTipoUsuario</t>
+  </si>
+  <si>
+    <t>nomeTipoUsuario</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>veterinário</t>
+  </si>
+  <si>
+    <t>pet</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>adm@adm.com</t>
+  </si>
+  <si>
+    <t>adm123</t>
+  </si>
+  <si>
+    <t>saulo@email.com</t>
+  </si>
+  <si>
+    <t>saulo123</t>
+  </si>
+  <si>
+    <t>caique@email.com</t>
+  </si>
+  <si>
+    <t>caique123</t>
+  </si>
+  <si>
+    <t>junior@email.com</t>
+  </si>
+  <si>
+    <t>junior123</t>
+  </si>
+  <si>
+    <t>loli@email.com</t>
+  </si>
+  <si>
+    <t>loli123</t>
+  </si>
+  <si>
+    <t>sammy@email.com</t>
+  </si>
+  <si>
+    <t>sammy123</t>
+  </si>
+  <si>
+    <t>situacao</t>
+  </si>
+  <si>
+    <t>idSituacao</t>
+  </si>
+  <si>
+    <t>nomeSituacao</t>
+  </si>
+  <si>
+    <t>realizada</t>
+  </si>
+  <si>
+    <t>agendada</t>
+  </si>
+  <si>
+    <t>cancelada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +271,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="23">
     <fill>
@@ -328,10 +423,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -343,9 +439,6 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -355,27 +448,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -385,9 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -398,9 +479,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -408,14 +486,40 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,42 +832,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D705F068-5948-47F4-B215-F29ECCA9317E}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="G1" s="36" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="G1" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -776,23 +883,26 @@
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -805,300 +915,513 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="31">
-        <v>1</v>
-      </c>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="26">
+        <v>1</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="27">
         <v>43383</v>
       </c>
-      <c r="J3" s="33">
-        <v>1</v>
-      </c>
-      <c r="K3" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G4" s="31">
-        <v>2</v>
-      </c>
-      <c r="H4" s="30" t="s">
+      <c r="J3" s="28">
+        <v>1</v>
+      </c>
+      <c r="K3" s="28">
+        <v>1</v>
+      </c>
+      <c r="L3" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G4" s="26">
+        <v>2</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="27">
         <v>42873</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="28">
         <v>4</v>
       </c>
-      <c r="K4" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="K4" s="28">
+        <v>1</v>
+      </c>
+      <c r="L4" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="G5" s="26">
+        <v>3</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="27">
+        <v>42537</v>
+      </c>
+      <c r="J5" s="28">
+        <v>1</v>
+      </c>
+      <c r="K5" s="28">
+        <v>2</v>
+      </c>
+      <c r="L5" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="G5" s="31">
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9">
+        <v>432551</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="D10" s="13">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9">
+        <v>653655</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="9">
         <v>3</v>
       </c>
-      <c r="H5" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="32">
-        <v>42537</v>
-      </c>
-      <c r="J5" s="33">
-        <v>1</v>
-      </c>
-      <c r="K5" s="33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="13">
+        <v>3</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G14" s="21">
+        <v>1</v>
+      </c>
+      <c r="H14" s="22">
+        <v>1</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="G15" s="21">
+        <v>2</v>
+      </c>
+      <c r="H15" s="22">
+        <v>2</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="21">
+        <v>3</v>
+      </c>
+      <c r="H16" s="22">
+        <v>2</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <v>1</v>
+      </c>
+      <c r="B17" s="22">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="21">
+        <v>4</v>
+      </c>
+      <c r="H17" s="22">
+        <v>3</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
+        <v>2</v>
+      </c>
+      <c r="B18" s="22">
+        <v>1</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="21">
+        <v>5</v>
+      </c>
+      <c r="H18" s="22">
+        <v>3</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="21">
+        <v>3</v>
+      </c>
+      <c r="B19" s="22">
+        <v>1</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="21">
+        <v>6</v>
+      </c>
+      <c r="H19" s="22">
+        <v>3</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="21">
+        <v>4</v>
+      </c>
+      <c r="B20" s="22">
+        <v>2</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="G22" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10">
-        <v>1</v>
-      </c>
-      <c r="C7" s="10">
-        <v>432551</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="10">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10">
-        <v>653655</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="D10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="G10" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="42" t="s">
+      <c r="I23" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J23" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="42" t="s">
+      <c r="K23" s="35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="15">
-        <v>1</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="20">
-        <v>1</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="38">
-        <v>1</v>
-      </c>
-      <c r="H12" s="39">
-        <v>1</v>
-      </c>
-      <c r="I12" s="39">
-        <v>1</v>
-      </c>
-      <c r="J12" s="37" t="s">
+      <c r="L23" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="32">
+        <v>1</v>
+      </c>
+      <c r="H24" s="33">
+        <v>1</v>
+      </c>
+      <c r="I24" s="33">
+        <v>1</v>
+      </c>
+      <c r="J24" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="40">
-        <v>44392</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="15">
-        <v>2</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="20">
-        <v>2</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="38">
-        <v>2</v>
-      </c>
-      <c r="H13" s="39">
-        <v>2</v>
-      </c>
-      <c r="I13" s="39">
-        <v>2</v>
-      </c>
-      <c r="J13" s="37" t="s">
+      <c r="K24" s="36">
+        <v>44392.666666666664</v>
+      </c>
+      <c r="L24" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="32">
+        <v>2</v>
+      </c>
+      <c r="H25" s="33">
+        <v>2</v>
+      </c>
+      <c r="I25" s="33">
+        <v>2</v>
+      </c>
+      <c r="J25" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="40">
-        <v>44393</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G14" s="38">
+      <c r="K25" s="36">
+        <v>44393.708333333336</v>
+      </c>
+      <c r="L25" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>3</v>
       </c>
-      <c r="H14" s="39">
-        <v>2</v>
-      </c>
-      <c r="I14" s="39">
-        <v>1</v>
-      </c>
-      <c r="J14" s="37" t="s">
+      <c r="B26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="32">
+        <v>3</v>
+      </c>
+      <c r="H26" s="33">
+        <v>2</v>
+      </c>
+      <c r="I26" s="33">
+        <v>1</v>
+      </c>
+      <c r="J26" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="40">
-        <v>44394</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <v>1</v>
-      </c>
-      <c r="B17" s="26">
-        <v>1</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
-        <v>2</v>
-      </c>
-      <c r="B18" s="26">
-        <v>1</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="K26" s="36">
+        <v>44394.416666666664</v>
+      </c>
+      <c r="L26" s="46">
         <v>3</v>
       </c>
-      <c r="B19" s="26">
-        <v>1</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
-        <v>4</v>
-      </c>
-      <c r="B20" s="26">
-        <v>2</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>24</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G10:K10"/>
+  <mergeCells count="10">
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G22:L22"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I14" r:id="rId1" xr:uid="{D2EF2F9D-2E73-4D09-AA40-E6588D1D6681}"/>
+    <hyperlink ref="I15" r:id="rId2" xr:uid="{8F6C3485-BA9F-420A-A24F-52D2BD6C69C6}"/>
+    <hyperlink ref="I16" r:id="rId3" xr:uid="{D19B6E90-6F59-4DE3-B9D2-CA016690E4C3}"/>
+    <hyperlink ref="I17" r:id="rId4" xr:uid="{8AB79D33-C079-4300-BBCC-496FC6661F55}"/>
+    <hyperlink ref="I18" r:id="rId5" xr:uid="{9FAEFDA2-B072-4EA4-8632-8839EA70BC07}"/>
+    <hyperlink ref="I19" r:id="rId6" xr:uid="{E86A168A-C46C-4F28-BDFF-577CB66D1EC6}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>